<commit_message>
Classification Model completed, predicted the values
</commit_message>
<xml_diff>
--- a/Classification_data.xlsx
+++ b/Classification_data.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="10">
+  <si>
+    <t>EXP_NO</t>
+  </si>
   <si>
     <t>RMS</t>
   </si>
@@ -49,13 +52,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -70,47 +81,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -129,6 +104,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -137,9 +127,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,13 +154,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,16 +188,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,8 +210,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,43 +234,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,139 +396,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,17 +443,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -476,8 +461,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,6 +506,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -521,183 +530,170 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,36 +1043,39 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="2:8">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1098,11 +1097,11 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3">
@@ -1124,11 +1123,11 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4">
@@ -1150,11 +1149,11 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5">
@@ -1176,11 +1175,11 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6">
@@ -1202,11 +1201,11 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7">
@@ -1228,11 +1227,11 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8">
@@ -1254,11 +1253,11 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9">
@@ -1280,11 +1279,11 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10">
@@ -1306,11 +1305,11 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1332,11 +1331,11 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1358,11 +1357,11 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1384,11 +1383,11 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14">
@@ -1410,11 +1409,11 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1436,11 +1435,11 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1462,11 +1461,11 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17">
@@ -1488,11 +1487,11 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18">
@@ -1514,11 +1513,11 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19">
@@ -1540,11 +1539,11 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20">
@@ -1566,11 +1565,11 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21">
@@ -1592,11 +1591,11 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22">
@@ -1618,11 +1617,11 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23">
@@ -1644,11 +1643,11 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24">
@@ -1670,11 +1669,11 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25">
@@ -1696,11 +1695,11 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26">
@@ -1722,11 +1721,11 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1748,11 +1747,11 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28">
@@ -1774,11 +1773,11 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29">
@@ -1800,11 +1799,11 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
       <c r="B30">
@@ -1826,11 +1825,11 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1852,11 +1851,11 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32">
@@ -1878,11 +1877,11 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
       <c r="B33">
@@ -1904,11 +1903,11 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34">
@@ -1930,11 +1929,11 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35">
@@ -1956,11 +1955,11 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36">
@@ -1982,11 +1981,11 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>35</v>
       </c>
       <c r="B37">
@@ -2008,11 +2007,11 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38">
@@ -2034,11 +2033,11 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>37</v>
       </c>
       <c r="B39">
@@ -2060,11 +2059,11 @@
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>38</v>
       </c>
       <c r="B40">
@@ -2086,11 +2085,11 @@
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>39</v>
       </c>
       <c r="B41">
@@ -2112,11 +2111,11 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>40</v>
       </c>
       <c r="B42">
@@ -2138,11 +2137,11 @@
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>41</v>
       </c>
       <c r="B43">
@@ -2164,11 +2163,11 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>42</v>
       </c>
       <c r="B44">
@@ -2190,11 +2189,11 @@
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>43</v>
       </c>
       <c r="B45">
@@ -2216,11 +2215,11 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>44</v>
       </c>
       <c r="B46">
@@ -2242,11 +2241,11 @@
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>45</v>
       </c>
       <c r="B47">
@@ -2268,11 +2267,11 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>46</v>
       </c>
       <c r="B48">
@@ -2294,11 +2293,11 @@
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>47</v>
       </c>
       <c r="B49">
@@ -2320,11 +2319,11 @@
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
       <c r="B50">
@@ -2346,11 +2345,11 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51">
@@ -2372,11 +2371,11 @@
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>50</v>
       </c>
       <c r="B52">
@@ -2398,11 +2397,11 @@
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>51</v>
       </c>
       <c r="B53">
@@ -2424,11 +2423,11 @@
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>52</v>
       </c>
       <c r="B54">
@@ -2450,11 +2449,11 @@
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>53</v>
       </c>
       <c r="B55">
@@ -2476,11 +2475,11 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>54</v>
       </c>
       <c r="B56">
@@ -2502,11 +2501,11 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>55</v>
       </c>
       <c r="B57">
@@ -2528,11 +2527,11 @@
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>56</v>
       </c>
       <c r="B58">
@@ -2554,11 +2553,11 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>57</v>
       </c>
       <c r="B59">
@@ -2580,11 +2579,11 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="B60">
@@ -2606,11 +2605,11 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>59</v>
       </c>
       <c r="B61">
@@ -2632,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>